<commit_message>
disable all exceptions, add few xlxs files
</commit_message>
<xml_diff>
--- a/urls/bosch_urls.xlsx
+++ b/urls/bosch_urls.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgFTDMBlqeSWnX7Eyp51HHbPIwy6w=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mi8YTVxTDPDWDlmL54ExYb+QbLEKQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="218">
   <si>
     <t>id</t>
   </si>
@@ -36,92 +36,647 @@
     <t>price_instr</t>
   </si>
   <si>
-    <t>58313</t>
-  </si>
-  <si>
-    <t>Шлифмашина угловая "GWS 17-125 CI" (Bosch)</t>
-  </si>
-  <si>
-    <t>https://stroybatinfo.ru/catalog/113/349208/</t>
-  </si>
-  <si>
-    <t>https://kirov.vseinstrumenti.ru/instrument/shlifmashiny/bolgarka_ushm/bosch/uglovaya_shlifmashina_bosch_gws_17-125_ci_0_601_795_0r2/</t>
-  </si>
-  <si>
-    <t>13067</t>
-  </si>
-  <si>
-    <t>Шлифмашина угловая "GWS 15-150 CIH" (Bosch)</t>
-  </si>
-  <si>
-    <t>https://stroybatinfo.ru/catalog/113/5860/</t>
+    <t>54161</t>
+  </si>
+  <si>
+    <t>Дрель алмазного сверления "GDB 180 WE" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/180/260622/</t>
   </si>
   <si>
     <t>nope</t>
   </si>
   <si>
-    <t>53758</t>
-  </si>
-  <si>
-    <t>Шлифмашина угловая "GWS 1400" (Bosch)</t>
-  </si>
-  <si>
-    <t>https://stroybatinfo.ru/catalog/113/346877/</t>
-  </si>
-  <si>
-    <t>https://kirov.vseinstrumenti.ru/instrument/shlifmashiny/bolgarka_ushm/bosch/uglovaya_shlifmashina_bosch_gws_1400_0_601_824_8r0/</t>
-  </si>
-  <si>
-    <t>55552</t>
-  </si>
-  <si>
-    <t>Шлифмашина угловая "GWS 13-125 CIE" (Bosch)</t>
-  </si>
-  <si>
-    <t>https://stroybatinfo.ru/catalog/113/262000/</t>
-  </si>
-  <si>
-    <t>https://kirov.vseinstrumenti.ru/instrument/shlifmashiny/bolgarka_ushm/bosch/ugloshlifmashina_bosch_gws_13-125_cie_0_601_794_0r2/</t>
-  </si>
-  <si>
-    <t>57137</t>
-  </si>
-  <si>
-    <t>Шлифмашина угловая "GWS 13-125 CI" (Bosch)</t>
-  </si>
-  <si>
-    <t>https://stroybatinfo.ru/catalog/113/263222/</t>
-  </si>
-  <si>
-    <t>54148</t>
-  </si>
-  <si>
-    <t>Шлифмашина угловая "GWS 11-125" (Bosch)</t>
-  </si>
-  <si>
-    <t>https://stroybatinfo.ru/catalog/113/260331/</t>
-  </si>
-  <si>
-    <t>https://kirov.vseinstrumenti.ru/instrument/shlifmashiny/bolgarka_ushm/bosch/uglovaya_shlifmashina_bosch_gws_11-125_0_601_792_0r0/</t>
-  </si>
-  <si>
-    <t>52305</t>
-  </si>
-  <si>
-    <t>Шлифмашина угловая "GWS 1000" (Bosch)</t>
-  </si>
-  <si>
-    <t>https://stroybatinfo.ru/catalog/113/346876/</t>
-  </si>
-  <si>
-    <t>https://kirov.vseinstrumenti.ru/instrument/shlifmashiny/bolgarka_ushm/bosch/uglovaya_shlifmashina_bosch_gws_1000_0_601_821_8r0/</t>
+    <t>4119</t>
+  </si>
+  <si>
+    <t>Резак акк. "GOP 14,4V-EC" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/1058/249468/</t>
+  </si>
+  <si>
+    <t>67955</t>
+  </si>
+  <si>
+    <t>Дрель "GBM 1600 RЕ" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/88/386738/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/dreli/bezudarnye/bosch/bezudarnaya_drel_bosch_gbm_1600_re_professional_0_601_1b0_000/</t>
+  </si>
+  <si>
+    <t>62923</t>
+  </si>
+  <si>
+    <t>Дрель "GBM 13-2 RE " (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/85/384787/</t>
+  </si>
+  <si>
+    <t>4118</t>
+  </si>
+  <si>
+    <t>Дрель "GBM 13 HRE" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/85/5749/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/dreli/bezudarnye/bosch/gbm_13_hre_0601049603/</t>
+  </si>
+  <si>
+    <t>21648</t>
+  </si>
+  <si>
+    <t>Дрель "GBM 10 RE" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/85/5747/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/dreli/bezudarnye/bosch/gbm_10_re_0601473600/</t>
+  </si>
+  <si>
+    <t>87250</t>
+  </si>
+  <si>
+    <t>Гайковерт акк. "GDX 18V-200 C" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/82/115501/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/gajkoverty/akkumulyatornye/bosch/akk-udarn-li-ion-18-v-gdx-18v-200-c-06019g4201/</t>
+  </si>
+  <si>
+    <t>63098</t>
+  </si>
+  <si>
+    <t>Гайковерт акк. "GDX 18 V-EC" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/82/379494/</t>
+  </si>
+  <si>
+    <t>72229</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/82/3655280/</t>
+  </si>
+  <si>
+    <t>74015</t>
+  </si>
+  <si>
+    <t>Гайковерт акк. "GDX 14 V-Li" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/82/4466351/</t>
+  </si>
+  <si>
+    <t>80590</t>
+  </si>
+  <si>
+    <t>Гайковерт акк. "GDR 180-LI" (Bosch) 18 В, 0-2800 об/мин, 160 Нм, наружный квадрат на 1/4", 2 Li-ion акк-ра 3 Ач, 1,7 кг, кейс</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/82/98985/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/gajkoverty/akkumulyatornye/bosch/gdr-180-li-0-601-9g5-120/</t>
+  </si>
+  <si>
+    <t>2185</t>
+  </si>
+  <si>
+    <t>Гайковерт "GDS 30" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/846/5745/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/gajkoverty/setevye/bosch/impulsniy_gaykovert_bosch_gds_30_0601435108/</t>
+  </si>
+  <si>
+    <t>4129</t>
+  </si>
+  <si>
+    <t>Бороздодел "GNF 65 A" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/115/5743/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/borozdodely_shtroborezy/bosch/borozdodel_bosch_gnf_65_ca_0601368708/</t>
+  </si>
+  <si>
+    <t>1629</t>
+  </si>
+  <si>
+    <t>Бороздодел "GNF 35 CA" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/115/61621/</t>
+  </si>
+  <si>
+    <t>70941</t>
+  </si>
+  <si>
+    <t>Адаптер "GAA 18 V-24" (Bosch) 2 выхода USB, для Li-Ion аккумуляторов Bosch 14,4-18 В, зарядный ток 2,4 А или 2x1,2 А, зажим для ремня, 125 г, 1600A00J61</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/771/6853112/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/akkumulyatornyj/zaryadnye-ustrojstva/bosch/bosch-usb-perehodnik-dlya-zaryadki-na-akkumulyator-18-v-gaa-18v-24-1600a00j61/</t>
+  </si>
+  <si>
+    <t>50398</t>
+  </si>
+  <si>
+    <t>Пила торцовочная "GCM 800 SJ"(Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/94/384525/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/pily/tortsovochnye/bosch/tortsovochnaya_pila_bosch_gcm_800_sj_0_601_b19_000/</t>
+  </si>
+  <si>
+    <t>18275</t>
+  </si>
+  <si>
+    <t>Пила дисковая "GKS 190" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/97/5807/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/pily/tsirkulyarnye_diskovye/bosch/bosch_gks_190_0601623000/</t>
+  </si>
+  <si>
+    <t>67745</t>
+  </si>
+  <si>
+    <t>Перфоратор акк. "GBH 36 VF-LI Plus" (Bosch) 3 режима., 36 V, 2 Li-Ion акк-ра., 4 Аh., 3,2 Дж., 0-940 об/мин., 0-4200 уд/мин, SDS+, система быстрой смены патрона, БЗП, 4,6 кг., L-Boxx. 0611907002</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/1056/386634/</t>
+  </si>
+  <si>
+    <t>60779</t>
+  </si>
+  <si>
+    <t>Перфоратор "GBH 8-45 D" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/92/328014/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/perforatory/sds-max/bosch/perforator_bosch_gbh_8-45_d_0_611_265_100/</t>
+  </si>
+  <si>
+    <t>14945</t>
+  </si>
+  <si>
+    <t>Перфоратор "GBH 5-40 DCE" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/92/5803/</t>
+  </si>
+  <si>
+    <t>21508</t>
+  </si>
+  <si>
+    <t>Перфоратор "GBH 4-32 DFR" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/25382/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/perforatory/sds-plus/bosch/gbh_4-32_dfr-s_0611332101/</t>
+  </si>
+  <si>
+    <t>17338</t>
+  </si>
+  <si>
+    <t>Перфоратор "GBH 3-28 DRE" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/5801/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/perforatory/sds-plus/bosch/gbh_3-28_dre_061123a000/</t>
+  </si>
+  <si>
+    <t>70142</t>
+  </si>
+  <si>
+    <t>Перфоратор "GBH 2-28" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/442136/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/perforatory/sds-plus/bosch/perforator-bosch-gbh-2-28-0.611.267.500/</t>
+  </si>
+  <si>
+    <t>89573</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/115649/</t>
+  </si>
+  <si>
+    <t>69248</t>
+  </si>
+  <si>
+    <t>Перфоратор "GBH 2-28 F" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/387507/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/perforatory/sds-plus/bosch/perforator-bosch-gbh-2-28-f-0.611.267.600/</t>
+  </si>
+  <si>
+    <t>884</t>
+  </si>
+  <si>
+    <t>Перфоратор "GBH 2-26 DRE" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/18660/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/perforatory/sds-plus/bosch/gbh_2-26_dre_0611253768/</t>
+  </si>
+  <si>
+    <t>1473</t>
+  </si>
+  <si>
+    <t>Перфоратор "GBH 2-26 DFR" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/5794/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/perforatory/sds-plus/bosch/gbh_2-26_dfr_0611254768/</t>
+  </si>
+  <si>
+    <t>80983</t>
+  </si>
+  <si>
+    <t>Ножовка сабельная акк. "GSA 12V-14" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/83/99594/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/akkumulyatornyj/pily/sabelnye/bosch/akkumulyatornaya_sabelnaya_nozhovka__bosch_gsa_10.8v-li_0.601.64l.902/</t>
+  </si>
+  <si>
+    <t>63101</t>
+  </si>
+  <si>
+    <t>Ножовка сабельная акк. "GSA 18 V-LI" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/83/379467/</t>
+  </si>
+  <si>
+    <t>28077</t>
+  </si>
+  <si>
+    <t>Ножовка сабельная "GSA 1100 E" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/99/88328/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/pily/sabelnye_elektronozhovki/bosch/bosch_gsa_1100_e_0.601.64c.800/</t>
+  </si>
+  <si>
+    <t>886</t>
+  </si>
+  <si>
+    <t>Отбойный молоток "GSH 11E" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/89/5784/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/otbojnye_molotki/sds-max/bosch/gsh_11_e_0611316708/</t>
+  </si>
+  <si>
+    <t>8245</t>
+  </si>
+  <si>
+    <t>Отбойный молоток "GSH 16-30" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/89/5785/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/otbojnye_molotki/shestigrannye/bosch/gsh_16-30_0611335100gsh_16-30/</t>
+  </si>
+  <si>
+    <t>12201</t>
+  </si>
+  <si>
+    <t>Перфоратор с пылеудалением "GBH 2-23 REA" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/5790/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/perforatory/sds-plus/bosch/gbh_2-23_rea_professional_0611250500/</t>
+  </si>
+  <si>
+    <t>23979</t>
+  </si>
+  <si>
+    <t>Перфоратор "GBH 2-20 D" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/5789/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/perforatory/sds-plus/bosch/gbh_2-20_d_061125a400/</t>
+  </si>
+  <si>
+    <t>54228</t>
+  </si>
+  <si>
+    <t>Перфоратор "GBH 12-52 D" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/92/346865/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/perforatory/sds-max/bosch/perforator_bosch_gbh_12-52_d_0_611_266_100/</t>
+  </si>
+  <si>
+    <t>66172</t>
+  </si>
+  <si>
+    <t>Пила дисковая "GKS 600" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/97/384024/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/pily/tsirkulyarnye-diskovye/bosch/gks-600-06016a9020/</t>
+  </si>
+  <si>
+    <t>79643</t>
+  </si>
+  <si>
+    <t>Лобзик "GST 700" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/87/101196/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/lobziki/bosch/gst-700-0-601-2a7-020/</t>
+  </si>
+  <si>
+    <t>60148</t>
+  </si>
+  <si>
+    <t>Пылесос универсальный "GAS 15 PS" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/151/346875/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/uborka/pylesosy/promyshlennye-stroitelnye/bosch/pylesos-bosch-gas-15-ps-06019e5100/</t>
+  </si>
+  <si>
+    <t>83348</t>
+  </si>
+  <si>
+    <t>Гайковерт акк. "GDS 250-LI" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/82/106562/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/gajkoverty/akkumulyatornye/bosch/gds-250-li-0-601-9g6-120/</t>
+  </si>
+  <si>
+    <t>89576</t>
+  </si>
+  <si>
+    <t>Перфоратор акк. "GBH 180 LI" (Bosch) 3 режима., 18 V., 2 Li-Ion акк-ра., 4 Аh., 1,7 Дж., 0-1800 об/мин., 0-4550 уд/мин, SDS+, в комплекте набор буров.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/1056/115650/</t>
+  </si>
+  <si>
+    <t>75926</t>
+  </si>
+  <si>
+    <t>Набор аккумуляторный "Гайковерт GDR120-Li + Шуруповерт GSR 120Li" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/83/101288/</t>
+  </si>
+  <si>
+    <t>62463</t>
+  </si>
+  <si>
+    <t>Рубанок "GHO 6500" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/982/373895/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/rubanki/bosch/gho-6500-0-601-596-000/</t>
+  </si>
+  <si>
+    <t>88043</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "GSR 180 LI" (Bosch) 2A</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/115278/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/shurupoverty/akkumulyatornye-dreli-shurupoverty/bezudarnye/bosch/akkumulyatornyj-shurupovert-bosch-gsr-180-li-0.601.9f8.120/</t>
+  </si>
+  <si>
+    <t>68446</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "GSR 180 LI" (Bosch) 1.5A</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/387085/</t>
+  </si>
+  <si>
+    <t>81257</t>
+  </si>
+  <si>
+    <t>Гайковерт акк. "GDX 180-LI" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/82/100283/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/gajkoverty/akkumulyatornye/bosch/gdx-180-li-0-601-9g5-220/</t>
+  </si>
+  <si>
+    <t>66976</t>
+  </si>
+  <si>
+    <t>Шлифмашина угловая "GWS 750-125" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/386800/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/shlifmashiny/bolgarka-ushm/bosch/uglovaya-shlifmashina-bosch-gws-750-125-0.601.394.0r3/</t>
+  </si>
+  <si>
+    <t>68445</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "GSR 140 LI" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/387084/</t>
+  </si>
+  <si>
+    <t>90150</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "GSR 120-LI" (Bosch) 12 V, 0-380/1300 об/мин, 2 Li-Ion акк-ра 2 Ah., 30 Нм, БЗП 10 мм, 0,8 кг, подсветка, кейс.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/115950/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/shurupoverty/akkumulyatornye-dreli/bezudarnye/bosch/gsr-120-li-0-601-9g8-020/</t>
+  </si>
+  <si>
+    <t>68793</t>
+  </si>
+  <si>
+    <t>Шуруповерт акк. "GSR 120-LI" (Bosch) 1.5A</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/387269/</t>
+  </si>
+  <si>
+    <t>62464</t>
+  </si>
+  <si>
+    <t>Отбойный молоток "GSH 501" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/89/379478/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/otbojnye-molotki/sds-max/bosch/gsh501-0-611-337-020/</t>
+  </si>
+  <si>
+    <t>87968</t>
+  </si>
+  <si>
+    <t>Фрезер "GKF 550" (Bosch) 550 Вт., 33000 об/мин., цанга 6 мм, 1,4 кг., в коробке.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/104/115134/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/frezery/drugie/bosch/gkf-550-0-601-6a0-020/</t>
+  </si>
+  <si>
+    <t>72792</t>
+  </si>
+  <si>
+    <t>Перфоратор "GBH 2-24 DFR" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/3655281/</t>
+  </si>
+  <si>
+    <t>48105</t>
+  </si>
+  <si>
+    <t>Дрель "GBM 6 RE" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/85/254694/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/dreli/bezudarnye/bosch/gbm_6_re_0601472600/</t>
+  </si>
+  <si>
+    <t>70544</t>
+  </si>
+  <si>
+    <t>Перфоратор "GBH 2-24 DRE" (Bosch)</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/91/3870721/</t>
+  </si>
+  <si>
+    <t>11601</t>
+  </si>
+  <si>
+    <t>Дрель ударная "GSB 13 RE" (Bosch) БЗП</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/86/5757/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/dreli/udarnye/bosch/gsb_13_re_bzp_0601217100/</t>
+  </si>
+  <si>
+    <t>14882</t>
+  </si>
+  <si>
+    <t>Дрель ударная "GSB 13 RE" (Bosch) ЗВП</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/86/5758/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/dreli/udarnye/bosch/gsb_13_re/</t>
+  </si>
+  <si>
+    <t>79179</t>
+  </si>
+  <si>
+    <t>Отвертка акк. "Bosch GO" (Bosch) 3,6 В, зарядка через Micro-USB, регулировка крутящего момента, индикатор заряда, реверс + набор бит.</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/81/95929/</t>
+  </si>
+  <si>
+    <t>62465</t>
+  </si>
+  <si>
+    <t>Ш/м угловая "GWS 660" (Bosch) Коробка</t>
+  </si>
+  <si>
+    <t>https://stroybatinfo.ru/catalog/113/373896/</t>
+  </si>
+  <si>
+    <t>https://kirov.vseinstrumenti.ru/instrument/shlifmashiny/bolgarka-ushm/bosch/uglovaya-shlifmashina-bosch-gws-660-0.601.375.08n/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -144,7 +699,6 @@
       <u/>
       <color rgb="FF0000FF"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -160,7 +714,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -178,13 +732,6 @@
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -438,7 +985,7 @@
       <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -453,750 +1000,975 @@
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>21</v>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="6" t="s">
+    </row>
+    <row r="9" ht="12.75" customHeight="1">
+      <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="2"/>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
+      <c r="A10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
+      <c r="A11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
+      <c r="A12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
+      <c r="A13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
+      <c r="A15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
+      <c r="A16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="2"/>
+      <c r="A18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
+      <c r="A19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
+      <c r="A20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
+      <c r="A21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
+      <c r="A22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="7"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
+      <c r="A23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="7"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
+      <c r="A24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="7"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="2"/>
+      <c r="A25" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="7"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="2"/>
+      <c r="A26" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="7"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
+      <c r="A27" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="7"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
+      <c r="A28" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
+      <c r="A29" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="7"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
+      <c r="A30" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="7"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
+      <c r="A31" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="7"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
+      <c r="A32" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="7"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="2"/>
+      <c r="A33" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="7"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="2"/>
+      <c r="A34" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="7"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
+      <c r="A35" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="7"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
+      <c r="A36" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="7"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
+      <c r="A37" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="7"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
+      <c r="A38" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="7"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
+      <c r="A39" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="7"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
+      <c r="A40" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="7"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
+      <c r="A41" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="7"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="2"/>
+      <c r="A42" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="7"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
+      <c r="A43" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="7"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
+      <c r="A44" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="45" ht="12.75" customHeight="1">
-      <c r="A45" s="7"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
+      <c r="A45" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="7"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
+      <c r="A46" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="47" ht="12.75" customHeight="1">
-      <c r="A47" s="7"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
+      <c r="A47" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="48" ht="12.75" customHeight="1">
-      <c r="A48" s="7"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="9"/>
+      <c r="A48" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="A49" s="7"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
+      <c r="A49" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="50" ht="12.75" customHeight="1">
-      <c r="A50" s="7"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
+      <c r="A50" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="51" ht="12.75" customHeight="1">
-      <c r="A51" s="7"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="9"/>
+      <c r="A51" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="52" ht="12.75" customHeight="1">
-      <c r="A52" s="7"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="2"/>
+      <c r="A52" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="7"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="2"/>
+      <c r="A53" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" s="3"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="2"/>
+      <c r="A54" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" s="7"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="2"/>
+      <c r="A55" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" s="7"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="9"/>
+      <c r="A56" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" s="7"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
+      <c r="A57" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="58" ht="12.75" customHeight="1">
-      <c r="A58" s="7"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="9"/>
+      <c r="A58" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="59" ht="12.75" customHeight="1">
-      <c r="A59" s="7"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="9"/>
+      <c r="A59" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="60" ht="12.75" customHeight="1">
-      <c r="A60" s="7"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="2"/>
+      <c r="A60" s="1"/>
     </row>
     <row r="61" ht="12.75" customHeight="1">
-      <c r="A61" s="7"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="9"/>
+      <c r="A61" s="1"/>
     </row>
     <row r="62" ht="12.75" customHeight="1">
-      <c r="A62" s="7"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
+      <c r="A62" s="1"/>
     </row>
     <row r="63" ht="12.75" customHeight="1">
-      <c r="A63" s="7"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="2"/>
+      <c r="A63" s="1"/>
     </row>
     <row r="64" ht="12.75" customHeight="1">
-      <c r="A64" s="7"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="2"/>
+      <c r="A64" s="1"/>
     </row>
     <row r="65" ht="12.75" customHeight="1">
-      <c r="A65" s="7"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="9"/>
+      <c r="A65" s="1"/>
     </row>
     <row r="66" ht="12.75" customHeight="1">
-      <c r="A66" s="7"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="2"/>
+      <c r="A66" s="1"/>
     </row>
     <row r="67" ht="12.75" customHeight="1">
-      <c r="A67" s="7"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="9"/>
+      <c r="A67" s="1"/>
     </row>
     <row r="68" ht="12.75" customHeight="1">
-      <c r="A68" s="7"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="9"/>
+      <c r="A68" s="1"/>
     </row>
     <row r="69" ht="12.75" customHeight="1">
-      <c r="A69" s="7"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="9"/>
+      <c r="A69" s="1"/>
     </row>
     <row r="70" ht="12.75" customHeight="1">
-      <c r="A70" s="7"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="2"/>
+      <c r="A70" s="1"/>
     </row>
     <row r="71" ht="12.75" customHeight="1">
-      <c r="A71" s="7"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="2"/>
+      <c r="A71" s="1"/>
     </row>
     <row r="72" ht="12.75" customHeight="1">
-      <c r="A72" s="7"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="2"/>
+      <c r="A72" s="1"/>
     </row>
     <row r="73" ht="12.75" customHeight="1">
-      <c r="A73" s="7"/>
-      <c r="B73" s="4"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="9"/>
+      <c r="A73" s="1"/>
     </row>
     <row r="74" ht="12.75" customHeight="1">
-      <c r="A74" s="7"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="9"/>
+      <c r="A74" s="1"/>
     </row>
     <row r="75" ht="12.75" customHeight="1">
-      <c r="A75" s="7"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="9"/>
+      <c r="A75" s="1"/>
     </row>
     <row r="76" ht="12.75" customHeight="1">
-      <c r="A76" s="7"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="2"/>
+      <c r="A76" s="1"/>
     </row>
     <row r="77" ht="12.75" customHeight="1">
-      <c r="A77" s="7"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="9"/>
+      <c r="A77" s="1"/>
     </row>
     <row r="78" ht="12.75" customHeight="1">
-      <c r="A78" s="7"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="9"/>
+      <c r="A78" s="1"/>
     </row>
     <row r="79" ht="12.75" customHeight="1">
-      <c r="A79" s="7"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="9"/>
+      <c r="A79" s="1"/>
     </row>
     <row r="80" ht="12.75" customHeight="1">
-      <c r="A80" s="7"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="2"/>
+      <c r="A80" s="1"/>
     </row>
     <row r="81" ht="12.75" customHeight="1">
-      <c r="A81" s="7"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="9"/>
+      <c r="A81" s="1"/>
     </row>
     <row r="82" ht="12.75" customHeight="1">
-      <c r="A82" s="7"/>
-      <c r="B82" s="4"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="2"/>
+      <c r="A82" s="1"/>
     </row>
     <row r="83" ht="12.75" customHeight="1">
-      <c r="A83" s="7"/>
-      <c r="B83" s="4"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="9"/>
+      <c r="A83" s="1"/>
     </row>
     <row r="84" ht="12.75" customHeight="1">
-      <c r="A84" s="7"/>
-      <c r="B84" s="4"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="9"/>
+      <c r="A84" s="1"/>
     </row>
     <row r="85" ht="12.75" customHeight="1">
-      <c r="A85" s="7"/>
-      <c r="B85" s="4"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="9"/>
+      <c r="A85" s="1"/>
     </row>
     <row r="86" ht="12.75" customHeight="1">
-      <c r="A86" s="7"/>
-      <c r="B86" s="4"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="2"/>
+      <c r="A86" s="1"/>
     </row>
     <row r="87" ht="12.75" customHeight="1">
-      <c r="A87" s="7"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="9"/>
+      <c r="A87" s="1"/>
     </row>
     <row r="88" ht="12.75" customHeight="1">
-      <c r="A88" s="7"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="9"/>
+      <c r="A88" s="1"/>
     </row>
     <row r="89" ht="12.75" customHeight="1">
-      <c r="A89" s="7"/>
-      <c r="B89" s="4"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="9"/>
+      <c r="A89" s="1"/>
     </row>
     <row r="90" ht="12.75" customHeight="1">
-      <c r="A90" s="7"/>
-      <c r="B90" s="4"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="9"/>
+      <c r="A90" s="1"/>
     </row>
     <row r="91" ht="12.75" customHeight="1">
-      <c r="A91" s="7"/>
-      <c r="B91" s="4"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="2"/>
+      <c r="A91" s="1"/>
     </row>
     <row r="92" ht="12.75" customHeight="1">
-      <c r="A92" s="7"/>
-      <c r="B92" s="4"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="9"/>
+      <c r="A92" s="1"/>
     </row>
     <row r="93" ht="12.75" customHeight="1">
-      <c r="A93" s="7"/>
-      <c r="B93" s="4"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="9"/>
+      <c r="A93" s="1"/>
     </row>
     <row r="94" ht="12.75" customHeight="1">
-      <c r="A94" s="7"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="9"/>
+      <c r="A94" s="1"/>
     </row>
     <row r="95" ht="12.75" customHeight="1">
-      <c r="A95" s="7"/>
-      <c r="B95" s="4"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="9"/>
+      <c r="A95" s="1"/>
     </row>
     <row r="96" ht="12.75" customHeight="1">
-      <c r="A96" s="7"/>
-      <c r="B96" s="4"/>
-      <c r="C96" s="8"/>
-      <c r="D96" s="9"/>
+      <c r="A96" s="1"/>
     </row>
     <row r="97" ht="12.75" customHeight="1">
-      <c r="A97" s="7"/>
-      <c r="B97" s="4"/>
-      <c r="C97" s="8"/>
-      <c r="D97" s="9"/>
+      <c r="A97" s="1"/>
     </row>
     <row r="98" ht="12.75" customHeight="1">
-      <c r="A98" s="7"/>
-      <c r="B98" s="4"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="9"/>
+      <c r="A98" s="1"/>
     </row>
     <row r="99" ht="12.75" customHeight="1">
-      <c r="A99" s="7"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="8"/>
-      <c r="D99" s="9"/>
+      <c r="A99" s="1"/>
     </row>
     <row r="100" ht="12.75" customHeight="1">
-      <c r="A100" s="7"/>
-      <c r="B100" s="4"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="9"/>
+      <c r="A100" s="1"/>
     </row>
     <row r="101" ht="12.75" customHeight="1">
-      <c r="A101" s="7"/>
-      <c r="B101" s="4"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="9"/>
+      <c r="A101" s="1"/>
     </row>
     <row r="102" ht="12.75" customHeight="1">
-      <c r="A102" s="7"/>
-      <c r="B102" s="4"/>
-      <c r="C102" s="8"/>
-      <c r="D102" s="2"/>
+      <c r="A102" s="1"/>
     </row>
     <row r="103" ht="12.75" customHeight="1">
-      <c r="A103" s="7"/>
-      <c r="B103" s="4"/>
-      <c r="C103" s="8"/>
-      <c r="D103" s="2"/>
+      <c r="A103" s="1"/>
     </row>
     <row r="104" ht="12.75" customHeight="1">
-      <c r="A104" s="7"/>
-      <c r="B104" s="4"/>
-      <c r="C104" s="8"/>
-      <c r="D104" s="9"/>
+      <c r="A104" s="1"/>
     </row>
     <row r="105" ht="12.75" customHeight="1">
-      <c r="A105" s="7"/>
-      <c r="B105" s="4"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="9"/>
+      <c r="A105" s="1"/>
     </row>
     <row r="106" ht="12.75" customHeight="1">
-      <c r="A106" s="7"/>
-      <c r="B106" s="4"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="2"/>
+      <c r="A106" s="1"/>
     </row>
     <row r="107" ht="12.75" customHeight="1">
-      <c r="A107" s="7"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="9"/>
+      <c r="A107" s="1"/>
     </row>
     <row r="108" ht="12.75" customHeight="1">
-      <c r="A108" s="7"/>
-      <c r="B108" s="4"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="9"/>
+      <c r="A108" s="1"/>
     </row>
     <row r="109" ht="12.75" customHeight="1">
-      <c r="A109" s="7"/>
-      <c r="B109" s="4"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="2"/>
+      <c r="A109" s="1"/>
     </row>
     <row r="110" ht="12.75" customHeight="1">
-      <c r="A110" s="7"/>
-      <c r="B110" s="4"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="9"/>
+      <c r="A110" s="1"/>
     </row>
     <row r="111" ht="12.75" customHeight="1">
-      <c r="A111" s="7"/>
-      <c r="B111" s="4"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="9"/>
+      <c r="A111" s="1"/>
     </row>
     <row r="112" ht="12.75" customHeight="1">
-      <c r="A112" s="7"/>
-      <c r="B112" s="4"/>
-      <c r="C112" s="8"/>
-      <c r="D112" s="9"/>
+      <c r="A112" s="1"/>
     </row>
     <row r="113" ht="12.75" customHeight="1">
-      <c r="A113" s="7"/>
-      <c r="B113" s="4"/>
-      <c r="C113" s="8"/>
-      <c r="D113" s="9"/>
+      <c r="A113" s="1"/>
     </row>
     <row r="114" ht="12.75" customHeight="1">
-      <c r="A114" s="7"/>
-      <c r="B114" s="4"/>
-      <c r="C114" s="8"/>
-      <c r="D114" s="2"/>
+      <c r="A114" s="1"/>
     </row>
     <row r="115" ht="12.75" customHeight="1">
-      <c r="A115" s="7"/>
-      <c r="B115" s="4"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="9"/>
+      <c r="A115" s="1"/>
     </row>
     <row r="116" ht="12.75" customHeight="1">
-      <c r="A116" s="7"/>
-      <c r="B116" s="4"/>
-      <c r="C116" s="8"/>
-      <c r="D116" s="2"/>
+      <c r="A116" s="1"/>
     </row>
     <row r="117" ht="12.75" customHeight="1">
-      <c r="A117" s="7"/>
-      <c r="B117" s="4"/>
-      <c r="C117" s="8"/>
-      <c r="D117" s="9"/>
+      <c r="A117" s="1"/>
     </row>
     <row r="118" ht="12.75" customHeight="1">
-      <c r="A118" s="7"/>
-      <c r="B118" s="4"/>
-      <c r="C118" s="8"/>
-      <c r="D118" s="9"/>
+      <c r="A118" s="1"/>
     </row>
     <row r="119" ht="12.75" customHeight="1">
-      <c r="A119" s="7"/>
-      <c r="B119" s="4"/>
-      <c r="C119" s="8"/>
-      <c r="D119" s="2"/>
+      <c r="A119" s="1"/>
     </row>
     <row r="120" ht="12.75" customHeight="1">
-      <c r="A120" s="7"/>
-      <c r="B120" s="4"/>
-      <c r="C120" s="8"/>
-      <c r="D120" s="9"/>
+      <c r="A120" s="1"/>
     </row>
     <row r="121" ht="12.75" customHeight="1">
       <c r="A121" s="1"/>
@@ -3627,204 +4399,106 @@
     </row>
     <row r="930" ht="12.75" customHeight="1">
       <c r="A930" s="1"/>
-    </row>
-    <row r="931" ht="12.75" customHeight="1">
-      <c r="A931" s="1"/>
-    </row>
-    <row r="932" ht="12.75" customHeight="1">
-      <c r="A932" s="1"/>
-    </row>
-    <row r="933" ht="12.75" customHeight="1">
-      <c r="A933" s="1"/>
-    </row>
-    <row r="934" ht="12.75" customHeight="1">
-      <c r="A934" s="1"/>
-    </row>
-    <row r="935" ht="12.75" customHeight="1">
-      <c r="A935" s="1"/>
-    </row>
-    <row r="936" ht="12.75" customHeight="1">
-      <c r="A936" s="1"/>
-    </row>
-    <row r="937" ht="12.75" customHeight="1">
-      <c r="A937" s="1"/>
-    </row>
-    <row r="938" ht="12.75" customHeight="1">
-      <c r="A938" s="1"/>
-    </row>
-    <row r="939" ht="12.75" customHeight="1">
-      <c r="A939" s="1"/>
-    </row>
-    <row r="940" ht="12.75" customHeight="1">
-      <c r="A940" s="1"/>
-    </row>
-    <row r="941" ht="12.75" customHeight="1">
-      <c r="A941" s="1"/>
-    </row>
-    <row r="942" ht="12.75" customHeight="1">
-      <c r="A942" s="1"/>
-    </row>
-    <row r="943" ht="12.75" customHeight="1">
-      <c r="A943" s="1"/>
-    </row>
-    <row r="944" ht="12.75" customHeight="1">
-      <c r="A944" s="1"/>
-    </row>
-    <row r="945" ht="12.75" customHeight="1">
-      <c r="A945" s="1"/>
-    </row>
-    <row r="946" ht="12.75" customHeight="1">
-      <c r="A946" s="1"/>
-    </row>
-    <row r="947" ht="12.75" customHeight="1">
-      <c r="A947" s="1"/>
-    </row>
-    <row r="948" ht="12.75" customHeight="1">
-      <c r="A948" s="1"/>
-    </row>
-    <row r="949" ht="12.75" customHeight="1">
-      <c r="A949" s="1"/>
-    </row>
-    <row r="950" ht="12.75" customHeight="1">
-      <c r="A950" s="1"/>
-    </row>
-    <row r="951" ht="12.75" customHeight="1">
-      <c r="A951" s="1"/>
-    </row>
-    <row r="952" ht="12.75" customHeight="1">
-      <c r="A952" s="1"/>
-    </row>
-    <row r="953" ht="12.75" customHeight="1">
-      <c r="A953" s="1"/>
-    </row>
-    <row r="954" ht="12.75" customHeight="1">
-      <c r="A954" s="1"/>
-    </row>
-    <row r="955" ht="12.75" customHeight="1">
-      <c r="A955" s="1"/>
-    </row>
-    <row r="956" ht="12.75" customHeight="1">
-      <c r="A956" s="1"/>
-    </row>
-    <row r="957" ht="12.75" customHeight="1">
-      <c r="A957" s="1"/>
-    </row>
-    <row r="958" ht="12.75" customHeight="1">
-      <c r="A958" s="1"/>
-    </row>
-    <row r="959" ht="12.75" customHeight="1">
-      <c r="A959" s="1"/>
-    </row>
-    <row r="960" ht="12.75" customHeight="1">
-      <c r="A960" s="1"/>
-    </row>
-    <row r="961" ht="12.75" customHeight="1">
-      <c r="A961" s="1"/>
-    </row>
-    <row r="962" ht="12.75" customHeight="1">
-      <c r="A962" s="1"/>
-    </row>
-    <row r="963" ht="12.75" customHeight="1">
-      <c r="A963" s="1"/>
-    </row>
-    <row r="964" ht="12.75" customHeight="1">
-      <c r="A964" s="1"/>
-    </row>
-    <row r="965" ht="12.75" customHeight="1">
-      <c r="A965" s="1"/>
-    </row>
-    <row r="966" ht="12.75" customHeight="1">
-      <c r="A966" s="1"/>
-    </row>
-    <row r="967" ht="12.75" customHeight="1">
-      <c r="A967" s="1"/>
-    </row>
-    <row r="968" ht="12.75" customHeight="1">
-      <c r="A968" s="1"/>
-    </row>
-    <row r="969" ht="12.75" customHeight="1">
-      <c r="A969" s="1"/>
-    </row>
-    <row r="970" ht="12.75" customHeight="1">
-      <c r="A970" s="1"/>
-    </row>
-    <row r="971" ht="12.75" customHeight="1">
-      <c r="A971" s="1"/>
-    </row>
-    <row r="972" ht="12.75" customHeight="1">
-      <c r="A972" s="1"/>
-    </row>
-    <row r="973" ht="12.75" customHeight="1">
-      <c r="A973" s="1"/>
-    </row>
-    <row r="974" ht="12.75" customHeight="1">
-      <c r="A974" s="1"/>
-    </row>
-    <row r="975" ht="12.75" customHeight="1">
-      <c r="A975" s="1"/>
-    </row>
-    <row r="976" ht="12.75" customHeight="1">
-      <c r="A976" s="1"/>
-    </row>
-    <row r="977" ht="12.75" customHeight="1">
-      <c r="A977" s="1"/>
-    </row>
-    <row r="978" ht="12.75" customHeight="1">
-      <c r="A978" s="1"/>
-    </row>
-    <row r="979" ht="12.75" customHeight="1">
-      <c r="A979" s="1"/>
-    </row>
-    <row r="980" ht="12.75" customHeight="1">
-      <c r="A980" s="1"/>
-    </row>
-    <row r="981" ht="12.75" customHeight="1">
-      <c r="A981" s="1"/>
-    </row>
-    <row r="982" ht="12.75" customHeight="1">
-      <c r="A982" s="1"/>
-    </row>
-    <row r="983" ht="12.75" customHeight="1">
-      <c r="A983" s="1"/>
-    </row>
-    <row r="984" ht="12.75" customHeight="1">
-      <c r="A984" s="1"/>
-    </row>
-    <row r="985" ht="12.75" customHeight="1">
-      <c r="A985" s="1"/>
-    </row>
-    <row r="986" ht="12.75" customHeight="1">
-      <c r="A986" s="1"/>
-    </row>
-    <row r="987" ht="12.75" customHeight="1">
-      <c r="A987" s="1"/>
-    </row>
-    <row r="988" ht="12.75" customHeight="1">
-      <c r="A988" s="1"/>
-    </row>
-    <row r="989" ht="12.75" customHeight="1">
-      <c r="A989" s="1"/>
-    </row>
-    <row r="990" ht="12.75" customHeight="1">
-      <c r="A990" s="1"/>
-    </row>
-    <row r="991" ht="12.75" customHeight="1">
-      <c r="A991" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="D2"/>
-    <hyperlink r:id="rId3" ref="C3"/>
-    <hyperlink r:id="rId4" ref="C4"/>
-    <hyperlink r:id="rId5" ref="D4"/>
-    <hyperlink r:id="rId6" ref="C5"/>
-    <hyperlink r:id="rId7" ref="D5"/>
-    <hyperlink r:id="rId8" ref="C6"/>
-    <hyperlink r:id="rId9" ref="C7"/>
-    <hyperlink r:id="rId10" ref="D7"/>
-    <hyperlink r:id="rId11" ref="C8"/>
-    <hyperlink r:id="rId12" ref="D8"/>
+    <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink r:id="rId3" ref="C4"/>
+    <hyperlink r:id="rId4" ref="D4"/>
+    <hyperlink r:id="rId5" ref="C5"/>
+    <hyperlink r:id="rId6" ref="C6"/>
+    <hyperlink r:id="rId7" ref="D6"/>
+    <hyperlink r:id="rId8" ref="C7"/>
+    <hyperlink r:id="rId9" ref="D7"/>
+    <hyperlink r:id="rId10" ref="C8"/>
+    <hyperlink r:id="rId11" ref="D8"/>
+    <hyperlink r:id="rId12" ref="C9"/>
+    <hyperlink r:id="rId13" ref="C10"/>
+    <hyperlink r:id="rId14" ref="C11"/>
+    <hyperlink r:id="rId15" ref="C12"/>
+    <hyperlink r:id="rId16" ref="D12"/>
+    <hyperlink r:id="rId17" ref="C13"/>
+    <hyperlink r:id="rId18" ref="D13"/>
+    <hyperlink r:id="rId19" ref="C14"/>
+    <hyperlink r:id="rId20" ref="D14"/>
+    <hyperlink r:id="rId21" ref="C15"/>
+    <hyperlink r:id="rId22" ref="C16"/>
+    <hyperlink r:id="rId23" ref="D16"/>
+    <hyperlink r:id="rId24" ref="C17"/>
+    <hyperlink r:id="rId25" ref="D17"/>
+    <hyperlink r:id="rId26" ref="C18"/>
+    <hyperlink r:id="rId27" ref="D18"/>
+    <hyperlink r:id="rId28" ref="C19"/>
+    <hyperlink r:id="rId29" ref="C20"/>
+    <hyperlink r:id="rId30" ref="D20"/>
+    <hyperlink r:id="rId31" ref="C21"/>
+    <hyperlink r:id="rId32" ref="C22"/>
+    <hyperlink r:id="rId33" ref="D22"/>
+    <hyperlink r:id="rId34" ref="C23"/>
+    <hyperlink r:id="rId35" ref="D23"/>
+    <hyperlink r:id="rId36" ref="C24"/>
+    <hyperlink r:id="rId37" ref="D24"/>
+    <hyperlink r:id="rId38" ref="C25"/>
+    <hyperlink r:id="rId39" ref="C26"/>
+    <hyperlink r:id="rId40" ref="D26"/>
+    <hyperlink r:id="rId41" ref="C27"/>
+    <hyperlink r:id="rId42" ref="D27"/>
+    <hyperlink r:id="rId43" ref="C28"/>
+    <hyperlink r:id="rId44" ref="D28"/>
+    <hyperlink r:id="rId45" ref="C29"/>
+    <hyperlink r:id="rId46" ref="D29"/>
+    <hyperlink r:id="rId47" ref="C30"/>
+    <hyperlink r:id="rId48" ref="C31"/>
+    <hyperlink r:id="rId49" ref="D31"/>
+    <hyperlink r:id="rId50" ref="C32"/>
+    <hyperlink r:id="rId51" ref="D32"/>
+    <hyperlink r:id="rId52" ref="C33"/>
+    <hyperlink r:id="rId53" ref="D33"/>
+    <hyperlink r:id="rId54" ref="C34"/>
+    <hyperlink r:id="rId55" ref="D34"/>
+    <hyperlink r:id="rId56" ref="C35"/>
+    <hyperlink r:id="rId57" ref="D35"/>
+    <hyperlink r:id="rId58" ref="C36"/>
+    <hyperlink r:id="rId59" ref="D36"/>
+    <hyperlink r:id="rId60" ref="C37"/>
+    <hyperlink r:id="rId61" ref="D37"/>
+    <hyperlink r:id="rId62" ref="C38"/>
+    <hyperlink r:id="rId63" ref="D38"/>
+    <hyperlink r:id="rId64" ref="C39"/>
+    <hyperlink r:id="rId65" ref="D39"/>
+    <hyperlink r:id="rId66" ref="C40"/>
+    <hyperlink r:id="rId67" ref="D40"/>
+    <hyperlink r:id="rId68" ref="C41"/>
+    <hyperlink r:id="rId69" ref="C42"/>
+    <hyperlink r:id="rId70" ref="C43"/>
+    <hyperlink r:id="rId71" ref="D43"/>
+    <hyperlink r:id="rId72" ref="C44"/>
+    <hyperlink r:id="rId73" ref="D44"/>
+    <hyperlink r:id="rId74" ref="C45"/>
+    <hyperlink r:id="rId75" ref="C46"/>
+    <hyperlink r:id="rId76" ref="D46"/>
+    <hyperlink r:id="rId77" ref="C47"/>
+    <hyperlink r:id="rId78" ref="D47"/>
+    <hyperlink r:id="rId79" ref="C48"/>
+    <hyperlink r:id="rId80" ref="C49"/>
+    <hyperlink r:id="rId81" ref="D49"/>
+    <hyperlink r:id="rId82" ref="C50"/>
+    <hyperlink r:id="rId83" ref="C51"/>
+    <hyperlink r:id="rId84" ref="D51"/>
+    <hyperlink r:id="rId85" ref="C52"/>
+    <hyperlink r:id="rId86" ref="D52"/>
+    <hyperlink r:id="rId87" ref="C53"/>
+    <hyperlink r:id="rId88" ref="C54"/>
+    <hyperlink r:id="rId89" ref="D54"/>
+    <hyperlink r:id="rId90" ref="C55"/>
+    <hyperlink r:id="rId91" ref="C56"/>
+    <hyperlink r:id="rId92" ref="D56"/>
+    <hyperlink r:id="rId93" ref="C57"/>
+    <hyperlink r:id="rId94" ref="D57"/>
+    <hyperlink r:id="rId95" ref="C58"/>
+    <hyperlink r:id="rId96" ref="C59"/>
+    <hyperlink r:id="rId97" ref="D59"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="1.05277777777778" footer="0.0" header="0.0" left="0.7875" right="0.7875" top="1.05277777777778"/>
@@ -3833,6 +4507,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId13"/>
+  <drawing r:id="rId98"/>
 </worksheet>
 </file>
</xml_diff>